<commit_message>
add word in order
</commit_message>
<xml_diff>
--- a/data/tasks.xlsx
+++ b/data/tasks.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2936"/>
+  <dimension ref="A1:F3138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10443,7 +10443,7 @@
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Растущий объем дохода приводит к росту инвестиций. ; Краткосрочная кривая совокупного предложения горизонтальна лишь до определенного момента. Далее она получает положительный наклон, приобретая тенденцию к восхождению: совокупное предложение возрастает с ростом цен. ; При росте предложения денег кривая LM сместится вправо, а равновесный уровень реального дохода возрастет.</t>
+          <t>Кривая совокупного спроса перемещается вверх и вправо. ; Кривая совокупного предложения принимает вид вертикальной прямой. ; Краткосрочная кривая совокупного предложения горизонтальна лишь до определенного момента. Далее она получает положительный наклон, приобретая тенденцию к восхождению: совокупное предложение возрастает с ростом цен.</t>
         </is>
       </c>
     </row>
@@ -10470,7 +10470,7 @@
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>Кривая совокупного предложения принимает вид вертикальной прямой. ; Кривая наклонена вниз. ; Более высокая ставка процента снижает планируемые инвестиции.</t>
+          <t>Кривая совокупного предложения принимает вид вертикальной прямой. ; Кривая совокупного спроса на труд наклонена вниз, показывая, что увеличение реальной заработной платы в экономике снижает общее количество труда, которое хотят использовать фирмы. ; Высокие темпы естественного демографического прироста приводят к снижению реальных доходов на душу населения.</t>
         </is>
       </c>
     </row>
@@ -10497,7 +10497,7 @@
       </c>
       <c r="F377" t="inlineStr">
         <is>
-          <t>Кривая предельных издержек возрастает. ; Растущий объем дохода приводит к росту инвестиций. ; Кривая совокупного спроса перемещается вверх и вправо.</t>
+          <t>Кривая предельных издержек возрастает. ; Кривая совокупного предложения принимает вид вертикальной прямой. ; При росте предложения денег кривая LM сместится вправо, а равновесный уровень реального дохода возрастет.</t>
         </is>
       </c>
     </row>
@@ -10524,7 +10524,7 @@
       </c>
       <c r="F378" t="inlineStr">
         <is>
-          <t>Кривая наклонена вниз. ; При росте предложения денег кривая LM сместится вправо, а равновесный уровень реального дохода возрастет. ; Кривая совокупного спроса перемещается вверх и вправо.</t>
+          <t>Кривая совокупного предложения принимает вид вертикальной прямой. ; Кривая совокупного спроса на труд наклонена вниз, показывая, что увеличение реальной заработной платы в экономике снижает общее количество труда, которое хотят использовать фирмы. ; Высокие темпы естественного демографического прироста приводят к снижению реальных доходов на душу населения.</t>
         </is>
       </c>
     </row>
@@ -10551,7 +10551,7 @@
       </c>
       <c r="F379" t="inlineStr">
         <is>
-          <t>При росте предложения денег кривая LM сместится вправо, а равновесный уровень реального дохода возрастет. ; Кривая LM сдвигается вверх. ; Кривая предельных издержек возрастает.</t>
+          <t>Увеличение инвестиций приводит к увеличению национального продукта или дохода. ; Кривая совокупного спроса перемещается вверх и вправо. ; Кривая предельных издержек возрастает.</t>
         </is>
       </c>
     </row>
@@ -10578,7 +10578,7 @@
       </c>
       <c r="F380" t="inlineStr">
         <is>
-          <t>Кривая совокупного спроса перемещается вверх и вправо. ; Краткосрочная кривая совокупного предложения горизонтальна лишь до определенного момента. Далее она получает положительный наклон, приобретая тенденцию к восхождению: совокупное предложение возрастает с ростом цен. ; Увеличение инвестиций приводит к увеличению национального продукта или дохода.</t>
+          <t>Кривая LM сдвигается вверх. ; Кривая совокупного предложения принимает вид вертикальной прямой. ; Растущий объем дохода приводит к росту инвестиций.</t>
         </is>
       </c>
     </row>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>Кривая LM сдвигается вверх. ; Более высокая ставка процента снижает планируемые инвестиции. ; Кривая предельного дохода продукта труда идет вниз.</t>
+          <t>Более высокая ставка процента снижает планируемые инвестиции. ; Кривая наклонена вниз. ; Кривая LM сдвигается вверх.</t>
         </is>
       </c>
     </row>
@@ -10632,7 +10632,7 @@
       </c>
       <c r="F382" t="inlineStr">
         <is>
-          <t>Увеличение инвестиций приводит к увеличению национального продукта или дохода. ; Растущий объем дохода приводит к росту инвестиций. ; Кривая совокупного спроса перемещается вверх и вправо.</t>
+          <t>При росте предложения денег кривая LM сместится вправо, а равновесный уровень реального дохода возрастет. ; Кривая LM сдвигается вверх. ; Увеличение инвестиций приводит к увеличению национального продукта или дохода.</t>
         </is>
       </c>
     </row>
@@ -10659,7 +10659,7 @@
       </c>
       <c r="F383" t="inlineStr">
         <is>
-          <t>Кривая наклонена вниз. ; Кривая предельного дохода продукта труда идет вниз. ; Увеличение инвестиций приводит к увеличению национального продукта или дохода.</t>
+          <t>Увеличение инвестиций приводит к увеличению национального продукта или дохода. ; Кривая наклонена вниз. ; Растущий объем дохода приводит к росту инвестиций.</t>
         </is>
       </c>
     </row>
@@ -10686,7 +10686,7 @@
       </c>
       <c r="F384" t="inlineStr">
         <is>
-          <t>Высокие темпы естественного демографического прироста приводят к снижению реальных доходов на душу населения. ; Кривая совокупного спроса перемещается вверх и вправо. ; Кривая предельного продукта труда имеет отрицательный наклон.</t>
+          <t>Кривая предельного продукта труда имеет отрицательный наклон. ; Кривая совокупного предложения принимает вид вертикальной прямой. ; Высокие темпы естественного демографического прироста приводят к снижению реальных доходов на душу населения.</t>
         </is>
       </c>
     </row>
@@ -10713,7 +10713,7 @@
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>Кривая совокупного спроса на труд наклонена вниз, показывая, что увеличение реальной заработной платы в экономике снижает общее количество труда, которое хотят использовать фирмы. ; Кривая совокупного спроса перемещается вверх и вправо. ; Кривая предельного дохода продукта труда идет вниз.</t>
+          <t>Кривая совокупного спроса на труд наклонена вниз, показывая, что увеличение реальной заработной платы в экономике снижает общее количество труда, которое хотят использовать фирмы. ; Кривая предельного дохода продукта труда идет вниз. ; Кривая наклонена вниз.</t>
         </is>
       </c>
     </row>
@@ -10740,7 +10740,7 @@
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>Кривая LM сдвигается вверх. ; Кривая совокупного предложения принимает вид вертикальной прямой. ; Кривая предельных издержек возрастает.</t>
+          <t>Кривая LM сдвигается вверх. ; Кривая совокупного спроса перемещается вверх и вправо. ; Кривая предельных издержек возрастает.</t>
         </is>
       </c>
     </row>
@@ -10767,7 +10767,7 @@
       </c>
       <c r="F387" t="inlineStr">
         <is>
-          <t>Кривая LM сдвигается вверх. ; Кривая предельного дохода продукта труда идет вниз. ; Более высокая ставка процента снижает планируемые инвестиции.</t>
+          <t>Кривая наклонена вниз. ; Растущий объем дохода приводит к росту инвестиций. ; Высокие темпы естественного демографического прироста приводят к снижению реальных доходов на душу населения.</t>
         </is>
       </c>
     </row>
@@ -10794,7 +10794,7 @@
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t>Кривая предельного дохода продукта труда идет вниз. ; Высокие темпы естественного демографического прироста приводят к снижению реальных доходов на душу населения. ; Кривая совокупного спроса на труд наклонена вниз, показывая, что увеличение реальной заработной платы в экономике снижает общее количество труда, которое хотят использовать фирмы.</t>
+          <t>Кривая предельного продукта труда имеет отрицательный наклон. ; Кривая совокупного предложения принимает вид вертикальной прямой. ; Кривая совокупного спроса перемещается вверх и вправо.</t>
         </is>
       </c>
     </row>
@@ -67571,6 +67571,4450 @@
       <c r="E2936" t="inlineStr">
         <is>
           <t>Поставить слово в правильную форму</t>
+        </is>
+      </c>
+    </row>
+    <row r="2937">
+      <c r="A2937" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2937" t="inlineStr">
+        <is>
+          <t>рост; номинальной; денежной; массы</t>
+        </is>
+      </c>
+      <c r="D2937" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2937" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2938">
+      <c r="A2938" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2938" t="inlineStr">
+        <is>
+          <t>рост; реальной; денежной; массы</t>
+        </is>
+      </c>
+      <c r="D2938" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2938" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2939">
+      <c r="A2939" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2939" t="inlineStr">
+        <is>
+          <t>увеличение; номинальной; денежной; массы</t>
+        </is>
+      </c>
+      <c r="D2939" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2939" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2940">
+      <c r="A2940" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2940" t="inlineStr">
+        <is>
+          <t>увеличение; реальной; денежной; массы</t>
+        </is>
+      </c>
+      <c r="D2940" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2940" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2941">
+      <c r="A2941" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2941" t="inlineStr">
+        <is>
+          <t>увеличение; темпа; роста; денежной; массы</t>
+        </is>
+      </c>
+      <c r="D2941" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2941" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2942">
+      <c r="A2942" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2942" t="inlineStr">
+        <is>
+          <t>увеличение; скорости; роста; денежной; массы</t>
+        </is>
+      </c>
+      <c r="D2942" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2942" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2943">
+      <c r="A2943" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2943" t="inlineStr">
+        <is>
+          <t>валютный; канал; денежной; трансмиссии</t>
+        </is>
+      </c>
+      <c r="D2943" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2943" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2944">
+      <c r="A2944" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2944" t="inlineStr">
+        <is>
+          <t>среднедушевые; денежные; доходы; населения</t>
+        </is>
+      </c>
+      <c r="D2944" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2944" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2945">
+      <c r="A2945" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2945" t="inlineStr">
+        <is>
+          <t>реальные; денежные; доходы; населения</t>
+        </is>
+      </c>
+      <c r="D2945" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2945" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2946">
+      <c r="A2946" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2946" t="inlineStr">
+        <is>
+          <t>реальные; располагаемые; денежные; доходы</t>
+        </is>
+      </c>
+      <c r="D2946" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2946" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2947">
+      <c r="A2947" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2947" t="inlineStr">
+        <is>
+          <t>трансмиссионный; механизм; денежно-кредитной; политики</t>
+        </is>
+      </c>
+      <c r="D2947" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2947" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2948">
+      <c r="A2948" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2948" t="inlineStr">
+        <is>
+          <t>балансовый; канал; денежно-кредитной; политики</t>
+        </is>
+      </c>
+      <c r="D2948" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2948" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2949">
+      <c r="A2949" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2949" t="inlineStr">
+        <is>
+          <t>неожиданные; шоки; денежно-кредитной; политики</t>
+        </is>
+      </c>
+      <c r="D2949" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2949" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2950">
+      <c r="A2950" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2950" t="inlineStr">
+        <is>
+          <t>асимметричное; влияние; денежно-кредитной; политики</t>
+        </is>
+      </c>
+      <c r="D2950" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2950" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2951">
+      <c r="A2951" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2951" t="inlineStr">
+        <is>
+          <t>эффекты; единой; денежно-кредитной; политики</t>
+        </is>
+      </c>
+      <c r="D2951" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2951" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2952">
+      <c r="A2952" t="inlineStr">
+        <is>
+          <t>денежный</t>
+        </is>
+      </c>
+      <c r="C2952" t="inlineStr">
+        <is>
+          <t>взаимные; фонды; денежного; рынка</t>
+        </is>
+      </c>
+      <c r="D2952" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2952" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2953">
+      <c r="A2953" t="inlineStr">
+        <is>
+          <t>заработный</t>
+        </is>
+      </c>
+      <c r="C2953" t="inlineStr">
+        <is>
+          <t>рост; реальной; заработной; платы</t>
+        </is>
+      </c>
+      <c r="D2953" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2953" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2954">
+      <c r="A2954" t="inlineStr">
+        <is>
+          <t>заработный</t>
+        </is>
+      </c>
+      <c r="C2954" t="inlineStr">
+        <is>
+          <t>в; виде; заработной; платы</t>
+        </is>
+      </c>
+      <c r="D2954" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2954" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2955">
+      <c r="A2955" t="inlineStr">
+        <is>
+          <t>инвестиционный</t>
+        </is>
+      </c>
+      <c r="C2955" t="inlineStr">
+        <is>
+          <t>инвестиционный; проект; по</t>
+        </is>
+      </c>
+      <c r="D2955" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2955" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2956">
+      <c r="A2956" t="inlineStr">
+        <is>
+          <t>инвестиционный</t>
+        </is>
+      </c>
+      <c r="C2956" t="inlineStr">
+        <is>
+          <t>оценка; эффективности; инвестиционных; проектов</t>
+        </is>
+      </c>
+      <c r="D2956" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2956" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2957">
+      <c r="A2957" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2957" t="inlineStr">
+        <is>
+          <t>доход; равен; предельным; издержкам</t>
+        </is>
+      </c>
+      <c r="D2957" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2957" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2958">
+      <c r="A2958" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2958" t="inlineStr">
+        <is>
+          <t>цена; равна; предельным; издержкам</t>
+        </is>
+      </c>
+      <c r="D2958" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2958" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2959">
+      <c r="A2959" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2959" t="inlineStr">
+        <is>
+          <t>цена; превышает; предельные; издержки</t>
+        </is>
+      </c>
+      <c r="D2959" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2959" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2960">
+      <c r="A2960" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2960" t="inlineStr">
+        <is>
+          <t>цена; выше; предельных; издержек</t>
+        </is>
+      </c>
+      <c r="D2960" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2960" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2961">
+      <c r="A2961" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2961" t="inlineStr">
+        <is>
+          <t>предельные; издержки; равны; цене</t>
+        </is>
+      </c>
+      <c r="D2961" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2961" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2962">
+      <c r="A2962" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2962" t="inlineStr">
+        <is>
+          <t>предельный; доход; равен; предельным; издержкам</t>
+        </is>
+      </c>
+      <c r="D2962" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2962" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2963">
+      <c r="A2963" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2963" t="inlineStr">
+        <is>
+          <t>предельный; доход; равняется; предельным; издержкам</t>
+        </is>
+      </c>
+      <c r="D2963" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2963" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2964">
+      <c r="A2964" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2964" t="inlineStr">
+        <is>
+          <t>предельная; норма; технического; замещения</t>
+        </is>
+      </c>
+      <c r="D2964" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2964" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2965">
+      <c r="A2965" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2965" t="inlineStr">
+        <is>
+          <t>предельная; норма; технологического; замещения</t>
+        </is>
+      </c>
+      <c r="D2965" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2965" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2966">
+      <c r="A2966" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2966" t="inlineStr">
+        <is>
+          <t>закон; убывающей; предельной; полезности</t>
+        </is>
+      </c>
+      <c r="D2966" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2966" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2967">
+      <c r="A2967" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2967" t="inlineStr">
+        <is>
+          <t>принцип; убывающей; предельной; полезности</t>
+        </is>
+      </c>
+      <c r="D2967" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2967" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2968">
+      <c r="A2968" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2968" t="inlineStr">
+        <is>
+          <t>предельный; доход; продукта; труда</t>
+        </is>
+      </c>
+      <c r="D2968" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2968" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2969">
+      <c r="A2969" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2969" t="inlineStr">
+        <is>
+          <t>предельный; продукт; труда; равен</t>
+        </is>
+      </c>
+      <c r="D2969" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2969" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2970">
+      <c r="A2970" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2970" t="inlineStr">
+        <is>
+          <t>кривая; предельного; продукта; труда</t>
+        </is>
+      </c>
+      <c r="D2970" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2970" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2971">
+      <c r="A2971" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2971" t="inlineStr">
+        <is>
+          <t>предельный; продукт; капитала; равен</t>
+        </is>
+      </c>
+      <c r="D2971" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2971" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2972">
+      <c r="A2972" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2972" t="inlineStr">
+        <is>
+          <t>закон; убывающей; предельной; производительности</t>
+        </is>
+      </c>
+      <c r="D2972" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2972" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2973">
+      <c r="A2973" t="inlineStr">
+        <is>
+          <t>предельный</t>
+        </is>
+      </c>
+      <c r="C2973" t="inlineStr">
+        <is>
+          <t>принцип; убывающей; предельной; производительности</t>
+        </is>
+      </c>
+      <c r="D2973" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2973" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2974">
+      <c r="A2974" t="inlineStr">
+        <is>
+          <t>процентный</t>
+        </is>
+      </c>
+      <c r="C2974" t="inlineStr">
+        <is>
+          <t>оценки; равновесной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D2974" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2974" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2975">
+      <c r="A2975" t="inlineStr">
+        <is>
+          <t>процентный</t>
+        </is>
+      </c>
+      <c r="C2975" t="inlineStr">
+        <is>
+          <t>мировая; реальная; процентная; ставка</t>
+        </is>
+      </c>
+      <c r="D2975" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2975" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2976">
+      <c r="A2976" t="inlineStr">
+        <is>
+          <t>процентный</t>
+        </is>
+      </c>
+      <c r="C2976" t="inlineStr">
+        <is>
+          <t>рост; реальной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D2976" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2976" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2977">
+      <c r="A2977" t="inlineStr">
+        <is>
+          <t>процентный</t>
+        </is>
+      </c>
+      <c r="C2977" t="inlineStr">
+        <is>
+          <t>увеличение; реальной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D2977" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2977" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2978">
+      <c r="A2978" t="inlineStr">
+        <is>
+          <t>процентный</t>
+        </is>
+      </c>
+      <c r="C2978" t="inlineStr">
+        <is>
+          <t>реальная; процентная; ставка; равна</t>
+        </is>
+      </c>
+      <c r="D2978" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2978" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2979">
+      <c r="A2979" t="inlineStr">
+        <is>
+          <t>процентный</t>
+        </is>
+      </c>
+      <c r="C2979" t="inlineStr">
+        <is>
+          <t>процентная; ставка,; обеспечивающая; равновесие</t>
+        </is>
+      </c>
+      <c r="D2979" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2979" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2980">
+      <c r="A2980" t="inlineStr">
+        <is>
+          <t>процентный</t>
+        </is>
+      </c>
+      <c r="C2980" t="inlineStr">
+        <is>
+          <t>значения; реальной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D2980" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2980" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2981">
+      <c r="A2981" t="inlineStr">
+        <is>
+          <t>процентный</t>
+        </is>
+      </c>
+      <c r="C2981" t="inlineStr">
+        <is>
+          <t>ожидаемая; реальная; процентная; ставка</t>
+        </is>
+      </c>
+      <c r="D2981" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2981" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2982">
+      <c r="A2982" t="inlineStr">
+        <is>
+          <t>процентный</t>
+        </is>
+      </c>
+      <c r="C2982" t="inlineStr">
+        <is>
+          <t>прогнозирование; чистой; процентной; маржи</t>
+        </is>
+      </c>
+      <c r="D2982" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2982" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2983">
+      <c r="A2983" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2983" t="inlineStr">
+        <is>
+          <t>темпы; прироста; реального; ввп</t>
+        </is>
+      </c>
+      <c r="D2983" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2983" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2984">
+      <c r="A2984" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2984" t="inlineStr">
+        <is>
+          <t>темпы; роста; реального; ввп</t>
+        </is>
+      </c>
+      <c r="D2984" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2984" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2985">
+      <c r="A2985" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2985" t="inlineStr">
+        <is>
+          <t>теория; реального; экономического; цикла</t>
+        </is>
+      </c>
+      <c r="D2985" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2985" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2986">
+      <c r="A2986" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2986" t="inlineStr">
+        <is>
+          <t>мировая; реальная; процентная; ставка</t>
+        </is>
+      </c>
+      <c r="D2986" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2986" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2987">
+      <c r="A2987" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2987" t="inlineStr">
+        <is>
+          <t>ожидаемая; реальная; процентная; ставка</t>
+        </is>
+      </c>
+      <c r="D2987" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2987" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2988">
+      <c r="A2988" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2988" t="inlineStr">
+        <is>
+          <t>рост; реальной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D2988" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2988" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2989">
+      <c r="A2989" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2989" t="inlineStr">
+        <is>
+          <t>увеличение; реальной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D2989" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2989" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2990">
+      <c r="A2990" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2990" t="inlineStr">
+        <is>
+          <t>значение; реальной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D2990" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2990" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2991">
+      <c r="A2991" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2991" t="inlineStr">
+        <is>
+          <t>реальная; ставка; процента; равна</t>
+        </is>
+      </c>
+      <c r="D2991" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2991" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2992">
+      <c r="A2992" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2992" t="inlineStr">
+        <is>
+          <t>рост; реальной; заработной; платы</t>
+        </is>
+      </c>
+      <c r="D2992" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2992" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2993">
+      <c r="A2993" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2993" t="inlineStr">
+        <is>
+          <t>уровень; реальной; заработной; платы</t>
+        </is>
+      </c>
+      <c r="D2993" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2993" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2994">
+      <c r="A2994" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2994" t="inlineStr">
+        <is>
+          <t>ставка; реальной; заработной; платы</t>
+        </is>
+      </c>
+      <c r="D2994" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2994" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2995">
+      <c r="A2995" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2995" t="inlineStr">
+        <is>
+          <t>увеличение; реальной; заработной; платы</t>
+        </is>
+      </c>
+      <c r="D2995" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2995" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2996">
+      <c r="A2996" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2996" t="inlineStr">
+        <is>
+          <t>снижение; реальной; заработной; платы</t>
+        </is>
+      </c>
+      <c r="D2996" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2996" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2997">
+      <c r="A2997" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2997" t="inlineStr">
+        <is>
+          <t>модернизация; реального; сектора; экономики</t>
+        </is>
+      </c>
+      <c r="D2997" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2997" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2998">
+      <c r="A2998" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2998" t="inlineStr">
+        <is>
+          <t>реальные; денежные; доходы; населения</t>
+        </is>
+      </c>
+      <c r="D2998" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2998" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="2999">
+      <c r="A2999" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C2999" t="inlineStr">
+        <is>
+          <t>реальные; располагаемые; денежные; доходы</t>
+        </is>
+      </c>
+      <c r="D2999" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E2999" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3000">
+      <c r="A3000" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C3000" t="inlineStr">
+        <is>
+          <t>величина; реального; предложения; денег</t>
+        </is>
+      </c>
+      <c r="D3000" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3000" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3001">
+      <c r="A3001" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C3001" t="inlineStr">
+        <is>
+          <t>реальные; диспропорции; экономического; пространства</t>
+        </is>
+      </c>
+      <c r="D3001" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3001" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3002">
+      <c r="A3002" t="inlineStr">
+        <is>
+          <t>реальный</t>
+        </is>
+      </c>
+      <c r="C3002" t="inlineStr">
+        <is>
+          <t>реальный; обменный; курс; рубля</t>
+        </is>
+      </c>
+      <c r="D3002" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3002" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3003">
+      <c r="A3003" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3003" t="inlineStr">
+        <is>
+          <t>кривая; долгосрочного; совокупного; предложения</t>
+        </is>
+      </c>
+      <c r="D3003" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3003" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3004">
+      <c r="A3004" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3004" t="inlineStr">
+        <is>
+          <t>кривая; краткосрочного; совокупного; предложения</t>
+        </is>
+      </c>
+      <c r="D3004" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3004" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3005">
+      <c r="A3005" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3005" t="inlineStr">
+        <is>
+          <t>долгосрочная; кривая; совокупного; предложения</t>
+        </is>
+      </c>
+      <c r="D3005" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3005" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3006">
+      <c r="A3006" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3006" t="inlineStr">
+        <is>
+          <t>краткосрочная; кривая; совокупного; предложения</t>
+        </is>
+      </c>
+      <c r="D3006" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3006" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3007">
+      <c r="A3007" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3007" t="inlineStr">
+        <is>
+          <t>сдвиг; кривой; совокупного; предложения; вправо</t>
+        </is>
+      </c>
+      <c r="D3007" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3007" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3008">
+      <c r="A3008" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3008" t="inlineStr">
+        <is>
+          <t>сдвиг; кривой; совокупного; предложения; влево</t>
+        </is>
+      </c>
+      <c r="D3008" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3008" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3009">
+      <c r="A3009" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3009" t="inlineStr">
+        <is>
+          <t>смещение; кривой; совокупного; предложения; вправо</t>
+        </is>
+      </c>
+      <c r="D3009" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3009" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3010">
+      <c r="A3010" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3010" t="inlineStr">
+        <is>
+          <t>смещение; кривой; совокупного; предложения; влево</t>
+        </is>
+      </c>
+      <c r="D3010" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3010" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3011">
+      <c r="A3011" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3011" t="inlineStr">
+        <is>
+          <t>кривая; совокупного; предложения; сдвигается; вправо</t>
+        </is>
+      </c>
+      <c r="D3011" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3011" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3012">
+      <c r="A3012" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3012" t="inlineStr">
+        <is>
+          <t>отрезок; кривой; совокупного; предложения</t>
+        </is>
+      </c>
+      <c r="D3012" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3012" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3013">
+      <c r="A3013" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3013" t="inlineStr">
+        <is>
+          <t>сдвиг; кривой; совокупного; спроса; вправо/влево</t>
+        </is>
+      </c>
+      <c r="D3013" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3013" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3014">
+      <c r="A3014" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3014" t="inlineStr">
+        <is>
+          <t>смещение; кривой; совокупного; спроса; вправо/влево</t>
+        </is>
+      </c>
+      <c r="D3014" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3014" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3015">
+      <c r="A3015" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3015" t="inlineStr">
+        <is>
+          <t>кривая; совокупного; спроса; смещается</t>
+        </is>
+      </c>
+      <c r="D3015" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3015" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3016">
+      <c r="A3016" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3016" t="inlineStr">
+        <is>
+          <t>сдвигает; кривую; совокупного; спроса</t>
+        </is>
+      </c>
+      <c r="D3016" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3016" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3017">
+      <c r="A3017" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3017" t="inlineStr">
+        <is>
+          <t>кривая; совокупного; спроса; сдвигается; вправо</t>
+        </is>
+      </c>
+      <c r="D3017" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3017" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3018">
+      <c r="A3018" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3018" t="inlineStr">
+        <is>
+          <t>уравнение; кривой; совокупного; спроса</t>
+        </is>
+      </c>
+      <c r="D3018" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3018" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3019">
+      <c r="A3019" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3019" t="inlineStr">
+        <is>
+          <t>отрицательный; наклон; кривой; совокупного; спроса</t>
+        </is>
+      </c>
+      <c r="D3019" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3019" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3020">
+      <c r="A3020" t="inlineStr">
+        <is>
+          <t>совокупный</t>
+        </is>
+      </c>
+      <c r="C3020" t="inlineStr">
+        <is>
+          <t>построение; модели; совокупных; расходов</t>
+        </is>
+      </c>
+      <c r="D3020" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3020" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3021">
+      <c r="A3021" t="inlineStr">
+        <is>
+          <t>финансовый</t>
+        </is>
+      </c>
+      <c r="C3021" t="inlineStr">
+        <is>
+          <t>финансовые; обязательства; перед</t>
+        </is>
+      </c>
+      <c r="D3021" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3021" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3022">
+      <c r="A3022" t="inlineStr">
+        <is>
+          <t>ценный</t>
+        </is>
+      </c>
+      <c r="C3022" t="inlineStr">
+        <is>
+          <t>доходность; рынка; ценных; бумаг</t>
+        </is>
+      </c>
+      <c r="D3022" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3022" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3023">
+      <c r="A3023" t="inlineStr">
+        <is>
+          <t>ценный</t>
+        </is>
+      </c>
+      <c r="C3023" t="inlineStr">
+        <is>
+          <t>операции; с; ценными; бумагами</t>
+        </is>
+      </c>
+      <c r="D3023" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3023" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3024">
+      <c r="A3024" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3024" t="inlineStr">
+        <is>
+          <t>уровень; цен; на</t>
+        </is>
+      </c>
+      <c r="D3024" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3024" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3025">
+      <c r="A3025" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3025" t="inlineStr">
+        <is>
+          <t>рост; общего; уровня; цен</t>
+        </is>
+      </c>
+      <c r="D3025" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3025" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3026">
+      <c r="A3026" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3026" t="inlineStr">
+        <is>
+          <t>изменение; общего; уровня; цен</t>
+        </is>
+      </c>
+      <c r="D3026" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3026" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3027">
+      <c r="A3027" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3027" t="inlineStr">
+        <is>
+          <t>равен; ожидаемому; уровню; цен</t>
+        </is>
+      </c>
+      <c r="D3027" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3027" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3028">
+      <c r="A3028" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3028" t="inlineStr">
+        <is>
+          <t>на; данном; уровне; цен</t>
+        </is>
+      </c>
+      <c r="D3028" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3028" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3029">
+      <c r="A3029" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3029" t="inlineStr">
+        <is>
+          <t>рост; цен; на</t>
+        </is>
+      </c>
+      <c r="D3029" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3029" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3030">
+      <c r="A3030" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3030" t="inlineStr">
+        <is>
+          <t>повышение; цен; на</t>
+        </is>
+      </c>
+      <c r="D3030" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3030" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3031">
+      <c r="A3031" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3031" t="inlineStr">
+        <is>
+          <t>снижение; цен; на</t>
+        </is>
+      </c>
+      <c r="D3031" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3031" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3032">
+      <c r="A3032" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3032" t="inlineStr">
+        <is>
+          <t>падение; цен; на</t>
+        </is>
+      </c>
+      <c r="D3032" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3032" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3033">
+      <c r="A3033" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3033" t="inlineStr">
+        <is>
+          <t>мировая; цена; на</t>
+        </is>
+      </c>
+      <c r="D3033" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3033" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3034">
+      <c r="A3034" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3034" t="inlineStr">
+        <is>
+          <t>средняя; цена; на</t>
+        </is>
+      </c>
+      <c r="D3034" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3034" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3035">
+      <c r="A3035" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3035" t="inlineStr">
+        <is>
+          <t>динамика; цен; на</t>
+        </is>
+      </c>
+      <c r="D3035" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3035" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3036">
+      <c r="A3036" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3036" t="inlineStr">
+        <is>
+          <t>шок; цен; на</t>
+        </is>
+      </c>
+      <c r="D3036" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3036" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3037">
+      <c r="A3037" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3037" t="inlineStr">
+        <is>
+          <t>внутренние; цены; на</t>
+        </is>
+      </c>
+      <c r="D3037" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3037" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3038">
+      <c r="A3038" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="C3038" t="inlineStr">
+        <is>
+          <t>реальная; цена; на</t>
+        </is>
+      </c>
+      <c r="D3038" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3038" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3039">
+      <c r="A3039" t="inlineStr">
+        <is>
+          <t>развитие</t>
+        </is>
+      </c>
+      <c r="C3039" t="inlineStr">
+        <is>
+          <t>индекс; развития; человеческого; потенциала</t>
+        </is>
+      </c>
+      <c r="D3039" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3039" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3040">
+      <c r="A3040" t="inlineStr">
+        <is>
+          <t>разница</t>
+        </is>
+      </c>
+      <c r="C3040" t="inlineStr">
+        <is>
+          <t>рассчитывается; как; разница; между</t>
+        </is>
+      </c>
+      <c r="D3040" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3040" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3041">
+      <c r="A3041" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3041" t="inlineStr">
+        <is>
+          <t>уравнение; кривой; совокупного; спроса</t>
+        </is>
+      </c>
+      <c r="D3041" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3041" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3042">
+      <c r="A3042" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3042" t="inlineStr">
+        <is>
+          <t>наклон; кривой; совокупного; спроса</t>
+        </is>
+      </c>
+      <c r="D3042" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3042" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3043">
+      <c r="A3043" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3043" t="inlineStr">
+        <is>
+          <t>сдвиг; кривой; совокупного; спроса</t>
+        </is>
+      </c>
+      <c r="D3043" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3043" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3044">
+      <c r="A3044" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3044" t="inlineStr">
+        <is>
+          <t>сдвигает; кривую; совокупного; спроса</t>
+        </is>
+      </c>
+      <c r="D3044" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3044" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3045">
+      <c r="A3045" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3045" t="inlineStr">
+        <is>
+          <t>кривая; совокупного; спроса; сдвигается; вправо/влево</t>
+        </is>
+      </c>
+      <c r="D3045" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3045" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3046">
+      <c r="A3046" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3046" t="inlineStr">
+        <is>
+          <t>кривая; совокупного; спроса; смещается; вправо/влево</t>
+        </is>
+      </c>
+      <c r="D3046" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3046" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3047">
+      <c r="A3047" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3047" t="inlineStr">
+        <is>
+          <t>точка; пересечения; кривых; спроса</t>
+        </is>
+      </c>
+      <c r="D3047" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3047" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3048">
+      <c r="A3048" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3048" t="inlineStr">
+        <is>
+          <t>общий; спрос; на; деньги</t>
+        </is>
+      </c>
+      <c r="D3048" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3048" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3049">
+      <c r="A3049" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3049" t="inlineStr">
+        <is>
+          <t>реальный; спрос; на; деньги</t>
+        </is>
+      </c>
+      <c r="D3049" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3049" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3050">
+      <c r="A3050" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3050" t="inlineStr">
+        <is>
+          <t>эластичность; спроса; по</t>
+        </is>
+      </c>
+      <c r="D3050" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3050" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3051">
+      <c r="A3051" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3051" t="inlineStr">
+        <is>
+          <t>эластичность; спроса; на</t>
+        </is>
+      </c>
+      <c r="D3051" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3051" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3052">
+      <c r="A3052" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3052" t="inlineStr">
+        <is>
+          <t>чувствительность; спроса; на; деньги</t>
+        </is>
+      </c>
+      <c r="D3052" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3052" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3053">
+      <c r="A3053" t="inlineStr">
+        <is>
+          <t>спрос</t>
+        </is>
+      </c>
+      <c r="C3053" t="inlineStr">
+        <is>
+          <t>эластичный; спрос; по; доходу</t>
+        </is>
+      </c>
+      <c r="D3053" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3053" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3054">
+      <c r="A3054" t="inlineStr">
+        <is>
+          <t>экономика</t>
+        </is>
+      </c>
+      <c r="C3054" t="inlineStr">
+        <is>
+          <t>модель; малой; открытой; экономики</t>
+        </is>
+      </c>
+      <c r="D3054" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3054" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3055">
+      <c r="A3055" t="inlineStr">
+        <is>
+          <t>экономика</t>
+        </is>
+      </c>
+      <c r="C3055" t="inlineStr">
+        <is>
+          <t>методы; оценки; теневой; экономики</t>
+        </is>
+      </c>
+      <c r="D3055" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3055" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3056">
+      <c r="A3056" t="inlineStr">
+        <is>
+          <t>экономика</t>
+        </is>
+      </c>
+      <c r="C3056" t="inlineStr">
+        <is>
+          <t>асимметрия; развития; цифровой; экономики</t>
+        </is>
+      </c>
+      <c r="D3056" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3056" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3057">
+      <c r="A3057" t="inlineStr">
+        <is>
+          <t>получить</t>
+        </is>
+      </c>
+      <c r="C3057" t="inlineStr">
+        <is>
+          <t>на; основе; полученных; _x000D_</t>
+        </is>
+      </c>
+      <c r="D3057" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3057" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3058">
+      <c r="A3058" t="inlineStr">
+        <is>
+          <t>ожидать</t>
+        </is>
+      </c>
+      <c r="C3058" t="inlineStr">
+        <is>
+          <t>ожидаемая; продолжительность; жизни; населения</t>
+        </is>
+      </c>
+      <c r="D3058" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3058" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3059">
+      <c r="A3059" t="inlineStr">
+        <is>
+          <t>ожидать</t>
+        </is>
+      </c>
+      <c r="C3059" t="inlineStr">
+        <is>
+          <t>ожидаемая; норма; чистой; прибыли</t>
+        </is>
+      </c>
+      <c r="D3059" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3059" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3060">
+      <c r="A3060" t="inlineStr">
+        <is>
+          <t>ожидать</t>
+        </is>
+      </c>
+      <c r="C3060" t="inlineStr">
+        <is>
+          <t>ожидаемая; реальная; процентная; ставка</t>
+        </is>
+      </c>
+      <c r="D3060" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3060" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3061">
+      <c r="A3061" t="inlineStr">
+        <is>
+          <t>показывать</t>
+        </is>
+      </c>
+      <c r="C3061" t="inlineStr">
+        <is>
+          <t>проведенный; анализ; показывает,; что</t>
+        </is>
+      </c>
+      <c r="D3061" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3061" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3062">
+      <c r="A3062" t="inlineStr">
+        <is>
+          <t>показывать</t>
+        </is>
+      </c>
+      <c r="C3062" t="inlineStr">
+        <is>
+          <t>мировой; опыт; показывает,; что</t>
+        </is>
+      </c>
+      <c r="D3062" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3062" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3063">
+      <c r="A3063" t="inlineStr">
+        <is>
+          <t>показывать</t>
+        </is>
+      </c>
+      <c r="C3063" t="inlineStr">
+        <is>
+          <t>мировая; практика; показывает,; что</t>
+        </is>
+      </c>
+      <c r="D3063" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3063" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3064">
+      <c r="A3064" t="inlineStr">
+        <is>
+          <t>показывать</t>
+        </is>
+      </c>
+      <c r="C3064" t="inlineStr">
+        <is>
+          <t>полученные; результаты; показывают,; что</t>
+        </is>
+      </c>
+      <c r="D3064" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3064" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3065">
+      <c r="A3065" t="inlineStr">
+        <is>
+          <t>показывать</t>
+        </is>
+      </c>
+      <c r="C3065" t="inlineStr">
+        <is>
+          <t>результаты; исследования; показывают,; что</t>
+        </is>
+      </c>
+      <c r="D3065" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3065" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3066">
+      <c r="A3066" t="inlineStr">
+        <is>
+          <t>показывать</t>
+        </is>
+      </c>
+      <c r="C3066" t="inlineStr">
+        <is>
+          <t>кривая; безразличия; показывает,; что</t>
+        </is>
+      </c>
+      <c r="D3066" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3066" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3067">
+      <c r="A3067" t="inlineStr">
+        <is>
+          <t>показывать</t>
+        </is>
+      </c>
+      <c r="C3067" t="inlineStr">
+        <is>
+          <t>кривая; Филлипса; показывает,; что</t>
+        </is>
+      </c>
+      <c r="D3067" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3067" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3068">
+      <c r="A3068" t="inlineStr">
+        <is>
+          <t>зависеть</t>
+        </is>
+      </c>
+      <c r="C3068" t="inlineStr">
+        <is>
+          <t>зависит; от; ставки; _x000D_</t>
+        </is>
+      </c>
+      <c r="D3068" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3068" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3069">
+      <c r="A3069" t="inlineStr">
+        <is>
+          <t>зависеть</t>
+        </is>
+      </c>
+      <c r="C3069" t="inlineStr">
+        <is>
+          <t>зависит; от; того,; что</t>
+        </is>
+      </c>
+      <c r="D3069" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3069" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3070">
+      <c r="A3070" t="inlineStr">
+        <is>
+          <t>зависеть</t>
+        </is>
+      </c>
+      <c r="C3070" t="inlineStr">
+        <is>
+          <t>во; многом; зависит; от</t>
+        </is>
+      </c>
+      <c r="D3070" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3070" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3071">
+      <c r="A3071" t="inlineStr">
+        <is>
+          <t>зависеть</t>
+        </is>
+      </c>
+      <c r="C3071" t="inlineStr">
+        <is>
+          <t>напрямую; зависит; от; _x000D_</t>
+        </is>
+      </c>
+      <c r="D3071" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3071" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3072">
+      <c r="A3072" t="inlineStr">
+        <is>
+          <t>зависеть</t>
+        </is>
+      </c>
+      <c r="C3072" t="inlineStr">
+        <is>
+          <t>в; значительной; степени; зависит</t>
+        </is>
+      </c>
+      <c r="D3072" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3072" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3073">
+      <c r="A3073" t="inlineStr">
+        <is>
+          <t>вести</t>
+        </is>
+      </c>
+      <c r="C3073" t="inlineStr">
+        <is>
+          <t>рост; дохода; ведет; к</t>
+        </is>
+      </c>
+      <c r="D3073" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3073" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3074">
+      <c r="A3074" t="inlineStr">
+        <is>
+          <t>вести</t>
+        </is>
+      </c>
+      <c r="C3074" t="inlineStr">
+        <is>
+          <t>ставка; процента; ведет; к</t>
+        </is>
+      </c>
+      <c r="D3074" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3074" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3075">
+      <c r="A3075" t="inlineStr">
+        <is>
+          <t>вести</t>
+        </is>
+      </c>
+      <c r="C3075" t="inlineStr">
+        <is>
+          <t>увеличение; ВВП; ведет; к</t>
+        </is>
+      </c>
+      <c r="D3075" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3075" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3076">
+      <c r="A3076" t="inlineStr">
+        <is>
+          <t>приводить</t>
+        </is>
+      </c>
+      <c r="C3076" t="inlineStr">
+        <is>
+          <t>в; свою; очередь; приводит; к</t>
+        </is>
+      </c>
+      <c r="D3076" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3076" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3077">
+      <c r="A3077" t="inlineStr">
+        <is>
+          <t>привести</t>
+        </is>
+      </c>
+      <c r="C3077" t="inlineStr">
+        <is>
+          <t>в; качестве; примера; можно; привести</t>
+        </is>
+      </c>
+      <c r="D3077" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3077" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3078">
+      <c r="A3078" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3078" t="inlineStr">
+        <is>
+          <t>высокий; уровень; экономического; развития</t>
+        </is>
+      </c>
+      <c r="D3078" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3078" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3079">
+      <c r="A3079" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3079" t="inlineStr">
+        <is>
+          <t>измерение; уровня; экономического; развития</t>
+        </is>
+      </c>
+      <c r="D3079" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3079" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3080">
+      <c r="A3080" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3080" t="inlineStr">
+        <is>
+          <t>механизмы; акселерации; социально-экономического; развития</t>
+        </is>
+      </c>
+      <c r="D3080" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3080" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3081">
+      <c r="A3081" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3081" t="inlineStr">
+        <is>
+          <t>реализации; стратегии; социально-экономического; развития</t>
+        </is>
+      </c>
+      <c r="D3081" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3081" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3082">
+      <c r="A3082" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3082" t="inlineStr">
+        <is>
+          <t>концепции; долгосрочного; социально-экономического; развития</t>
+        </is>
+      </c>
+      <c r="D3082" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3082" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3083">
+      <c r="A3083" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3083" t="inlineStr">
+        <is>
+          <t>стратегическое; планирование; социально-экономического; развития</t>
+        </is>
+      </c>
+      <c r="D3083" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3083" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3084">
+      <c r="A3084" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3084" t="inlineStr">
+        <is>
+          <t>на; основе; уровней; социально-экономического; развития</t>
+        </is>
+      </c>
+      <c r="D3084" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3084" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3085">
+      <c r="A3085" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3085" t="inlineStr">
+        <is>
+          <t>работы; классиков; экономической; теории</t>
+        </is>
+      </c>
+      <c r="D3085" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3085" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3086">
+      <c r="A3086" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3086" t="inlineStr">
+        <is>
+          <t>теория; реального; экономического; цикла</t>
+        </is>
+      </c>
+      <c r="D3086" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3086" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3087">
+      <c r="A3087" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3087" t="inlineStr">
+        <is>
+          <t>высокие; темпы; экономического; роста</t>
+        </is>
+      </c>
+      <c r="D3087" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3087" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3088">
+      <c r="A3088" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3088" t="inlineStr">
+        <is>
+          <t>новая; модель; экономического; роста</t>
+        </is>
+      </c>
+      <c r="D3088" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3088" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3089">
+      <c r="A3089" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3089" t="inlineStr">
+        <is>
+          <t>национальная; модель; экономического; роста</t>
+        </is>
+      </c>
+      <c r="D3089" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3089" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3090">
+      <c r="A3090" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3090" t="inlineStr">
+        <is>
+          <t>стимулирование; инновационного; экономического; роста</t>
+        </is>
+      </c>
+      <c r="D3090" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3090" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3091">
+      <c r="A3091" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3091" t="inlineStr">
+        <is>
+          <t>экономическая; оценка; эффективности; инвестиций</t>
+        </is>
+      </c>
+      <c r="D3091" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3091" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3092">
+      <c r="A3092" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3092" t="inlineStr">
+        <is>
+          <t>пространственная; связность; экономической; активности; с</t>
+        </is>
+      </c>
+      <c r="D3092" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3092" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3093">
+      <c r="A3093" t="inlineStr">
+        <is>
+          <t>экономический</t>
+        </is>
+      </c>
+      <c r="C3093" t="inlineStr">
+        <is>
+          <t>спецификация; макроэкономических; целевых; параметров</t>
+        </is>
+      </c>
+      <c r="D3093" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3093" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3094">
+      <c r="A3094" t="inlineStr">
+        <is>
+          <t>государственный</t>
+        </is>
+      </c>
+      <c r="C3094" t="inlineStr">
+        <is>
+          <t>увеличение; объемов; государственных; закупок</t>
+        </is>
+      </c>
+      <c r="D3094" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3094" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3095">
+      <c r="A3095" t="inlineStr">
+        <is>
+          <t>государственный</t>
+        </is>
+      </c>
+      <c r="C3095" t="inlineStr">
+        <is>
+          <t>государственное; регулирование; территориального; развития</t>
+        </is>
+      </c>
+      <c r="D3095" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3095" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3096">
+      <c r="A3096" t="inlineStr">
+        <is>
+          <t>государственный</t>
+        </is>
+      </c>
+      <c r="C3096" t="inlineStr">
+        <is>
+          <t>федеральная; служба; государственной; статистики</t>
+        </is>
+      </c>
+      <c r="D3096" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3096" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3097">
+      <c r="A3097" t="inlineStr">
+        <is>
+          <t>государственный</t>
+        </is>
+      </c>
+      <c r="C3097" t="inlineStr">
+        <is>
+          <t>финансирование; дефицита; государственного; бюджета</t>
+        </is>
+      </c>
+      <c r="D3097" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3097" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3098">
+      <c r="A3098" t="inlineStr">
+        <is>
+          <t>государственный</t>
+        </is>
+      </c>
+      <c r="C3098" t="inlineStr">
+        <is>
+          <t>исполнительные; органы; государственной; власти</t>
+        </is>
+      </c>
+      <c r="D3098" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3098" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3099">
+      <c r="A3099" t="inlineStr">
+        <is>
+          <t>государственный</t>
+        </is>
+      </c>
+      <c r="C3099" t="inlineStr">
+        <is>
+          <t>полномочия; органов; государственной; власти</t>
+        </is>
+      </c>
+      <c r="D3099" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3099" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3100">
+      <c r="A3100" t="inlineStr">
+        <is>
+          <t>государственный</t>
+        </is>
+      </c>
+      <c r="C3100" t="inlineStr">
+        <is>
+          <t>новая; модель; государственного; управления</t>
+        </is>
+      </c>
+      <c r="D3100" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3100" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3101">
+      <c r="A3101" t="inlineStr">
+        <is>
+          <t>государственный</t>
+        </is>
+      </c>
+      <c r="C3101" t="inlineStr">
+        <is>
+          <t>государственная; поддержка; нефтегазохимических; кластеров</t>
+        </is>
+      </c>
+      <c r="D3101" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3101" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3102">
+      <c r="A3102" t="inlineStr">
+        <is>
+          <t>средний</t>
+        </is>
+      </c>
+      <c r="C3102" t="inlineStr">
+        <is>
+          <t>в; среднем; по; стране</t>
+        </is>
+      </c>
+      <c r="D3102" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3102" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3103">
+      <c r="A3103" t="inlineStr">
+        <is>
+          <t>средний</t>
+        </is>
+      </c>
+      <c r="C3103" t="inlineStr">
+        <is>
+          <t>в; среднем; на; душу; населения</t>
+        </is>
+      </c>
+      <c r="D3103" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3103" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3104">
+      <c r="A3104" t="inlineStr">
+        <is>
+          <t>средний</t>
+        </is>
+      </c>
+      <c r="C3104" t="inlineStr">
+        <is>
+          <t>в; среднем; за; год</t>
+        </is>
+      </c>
+      <c r="D3104" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3104" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3105">
+      <c r="A3105" t="inlineStr">
+        <is>
+          <t>мировой</t>
+        </is>
+      </c>
+      <c r="C3105" t="inlineStr">
+        <is>
+          <t>мировая; реальная; процентная; ставка</t>
+        </is>
+      </c>
+      <c r="D3105" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3105" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3106">
+      <c r="A3106" t="inlineStr">
+        <is>
+          <t>мировой</t>
+        </is>
+      </c>
+      <c r="C3106" t="inlineStr">
+        <is>
+          <t>развитие; мировых; финансовых; институтов</t>
+        </is>
+      </c>
+      <c r="D3106" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3106" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3107">
+      <c r="A3107" t="inlineStr">
+        <is>
+          <t>мировой</t>
+        </is>
+      </c>
+      <c r="C3107" t="inlineStr">
+        <is>
+          <t>падение; мировых; цен; на</t>
+        </is>
+      </c>
+      <c r="D3107" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3107" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3108">
+      <c r="A3108" t="inlineStr">
+        <is>
+          <t>налоговый</t>
+        </is>
+      </c>
+      <c r="C3108" t="inlineStr">
+        <is>
+          <t>инструменты; налогового; стимулирования; _x000D_</t>
+        </is>
+      </c>
+      <c r="D3108" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3108" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3109">
+      <c r="A3109" t="inlineStr">
+        <is>
+          <t>рынок</t>
+        </is>
+      </c>
+      <c r="C3109" t="inlineStr">
+        <is>
+          <t>рынок; новых; фирм; _x000D_</t>
+        </is>
+      </c>
+      <c r="D3109" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3109" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3110">
+      <c r="A3110" t="inlineStr">
+        <is>
+          <t>ставка</t>
+        </is>
+      </c>
+      <c r="C3110" t="inlineStr">
+        <is>
+          <t>ставка; реальной; заработной; платы</t>
+        </is>
+      </c>
+      <c r="D3110" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3110" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3111">
+      <c r="A3111" t="inlineStr">
+        <is>
+          <t>ставка</t>
+        </is>
+      </c>
+      <c r="C3111" t="inlineStr">
+        <is>
+          <t>ставка; процента; равна; нулю</t>
+        </is>
+      </c>
+      <c r="D3111" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3111" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3112">
+      <c r="A3112" t="inlineStr">
+        <is>
+          <t>ставка</t>
+        </is>
+      </c>
+      <c r="C3112" t="inlineStr">
+        <is>
+          <t>рост; реальной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D3112" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3112" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3113">
+      <c r="A3113" t="inlineStr">
+        <is>
+          <t>ставка</t>
+        </is>
+      </c>
+      <c r="C3113" t="inlineStr">
+        <is>
+          <t>эффект; переноса; ключевой; ставки</t>
+        </is>
+      </c>
+      <c r="D3113" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3113" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3114">
+      <c r="A3114" t="inlineStr">
+        <is>
+          <t>ставка</t>
+        </is>
+      </c>
+      <c r="C3114" t="inlineStr">
+        <is>
+          <t>увеличение; реальной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D3114" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3114" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3115">
+      <c r="A3115" t="inlineStr">
+        <is>
+          <t>ставка</t>
+        </is>
+      </c>
+      <c r="C3115" t="inlineStr">
+        <is>
+          <t>значения; реальной; процентной; ставки</t>
+        </is>
+      </c>
+      <c r="D3115" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3115" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3116">
+      <c r="A3116" t="inlineStr">
+        <is>
+          <t>товар</t>
+        </is>
+      </c>
+      <c r="C3116" t="inlineStr">
+        <is>
+          <t>экспорт; товаров; за; границу</t>
+        </is>
+      </c>
+      <c r="D3116" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3116" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3117">
+      <c r="A3117" t="inlineStr">
+        <is>
+          <t>товар</t>
+        </is>
+      </c>
+      <c r="C3117" t="inlineStr">
+        <is>
+          <t>выпуск; товаров; для; внутреннего; потребления</t>
+        </is>
+      </c>
+      <c r="D3117" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3117" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3118">
+      <c r="A3118" t="inlineStr">
+        <is>
+          <t>товар</t>
+        </is>
+      </c>
+      <c r="C3118" t="inlineStr">
+        <is>
+          <t>импорт; товаров; на; внешние; рынки</t>
+        </is>
+      </c>
+      <c r="D3118" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3118" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3119">
+      <c r="A3119" t="inlineStr">
+        <is>
+          <t>товар</t>
+        </is>
+      </c>
+      <c r="C3119" t="inlineStr">
+        <is>
+          <t>альтернативное; приобретение; товаров; для; перепродажи</t>
+        </is>
+      </c>
+      <c r="D3119" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3119" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3120">
+      <c r="A3120" t="inlineStr">
+        <is>
+          <t>товар</t>
+        </is>
+      </c>
+      <c r="C3120" t="inlineStr">
+        <is>
+          <t>рыночная; стоимость; товаров; и; услуг</t>
+        </is>
+      </c>
+      <c r="D3120" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3120" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3121">
+      <c r="A3121" t="inlineStr">
+        <is>
+          <t>товар</t>
+        </is>
+      </c>
+      <c r="C3121" t="inlineStr">
+        <is>
+          <t>цена; за; единицу; товара</t>
+        </is>
+      </c>
+      <c r="D3121" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3121" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3122">
+      <c r="A3122" t="inlineStr">
+        <is>
+          <t>фактор</t>
+        </is>
+      </c>
+      <c r="C3122" t="inlineStr">
+        <is>
+          <t>факторы; развития; межбюджетных; отношений</t>
+        </is>
+      </c>
+      <c r="D3122" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3122" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3123">
+      <c r="A3123" t="inlineStr">
+        <is>
+          <t>фактор</t>
+        </is>
+      </c>
+      <c r="C3123" t="inlineStr">
+        <is>
+          <t>ключевые; факторы; оценки; должностей</t>
+        </is>
+      </c>
+      <c r="D3123" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3123" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3124">
+      <c r="A3124" t="inlineStr">
+        <is>
+          <t>фактор</t>
+        </is>
+      </c>
+      <c r="C3124" t="inlineStr">
+        <is>
+          <t>фактор; укрепления; межгосударственных; отношений</t>
+        </is>
+      </c>
+      <c r="D3124" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3124" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3125">
+      <c r="A3125" t="inlineStr">
+        <is>
+          <t>фактор</t>
+        </is>
+      </c>
+      <c r="C3125" t="inlineStr">
+        <is>
+          <t>факторы; вызывающие; сдвиг; кривой</t>
+        </is>
+      </c>
+      <c r="D3125" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3125" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3126">
+      <c r="A3126" t="inlineStr">
+        <is>
+          <t>фактор</t>
+        </is>
+      </c>
+      <c r="C3126" t="inlineStr">
+        <is>
+          <t>факторы; влияющие; на</t>
+        </is>
+      </c>
+      <c r="D3126" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3126" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3127">
+      <c r="A3127" t="inlineStr">
+        <is>
+          <t>инфляция</t>
+        </is>
+      </c>
+      <c r="C3127" t="inlineStr">
+        <is>
+          <t>выбор; между; инфляцией; и</t>
+        </is>
+      </c>
+      <c r="D3127" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3127" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3128">
+      <c r="A3128" t="inlineStr">
+        <is>
+          <t>инфляция</t>
+        </is>
+      </c>
+      <c r="C3128" t="inlineStr">
+        <is>
+          <t>зависимость; между; инфляцией; и</t>
+        </is>
+      </c>
+      <c r="D3128" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3128" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3129">
+      <c r="A3129" t="inlineStr">
+        <is>
+          <t>инфляция</t>
+        </is>
+      </c>
+      <c r="C3129" t="inlineStr">
+        <is>
+          <t>влияние; волатильности; инфляции; на</t>
+        </is>
+      </c>
+      <c r="D3129" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3129" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3130">
+      <c r="A3130" t="inlineStr">
+        <is>
+          <t>влиять</t>
+        </is>
+      </c>
+      <c r="C3130" t="inlineStr">
+        <is>
+          <t>факторы; внешней; среды; влияющие</t>
+        </is>
+      </c>
+      <c r="D3130" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3130" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3131">
+      <c r="A3131" t="inlineStr">
+        <is>
+          <t>влиять</t>
+        </is>
+      </c>
+      <c r="C3131" t="inlineStr">
+        <is>
+          <t>влиять; друг; на; друга</t>
+        </is>
+      </c>
+      <c r="D3131" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3131" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3132">
+      <c r="A3132" t="inlineStr">
+        <is>
+          <t>влиять</t>
+        </is>
+      </c>
+      <c r="C3132" t="inlineStr">
+        <is>
+          <t>никак; не; влиять; на</t>
+        </is>
+      </c>
+      <c r="D3132" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3132" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3133">
+      <c r="A3133" t="inlineStr">
+        <is>
+          <t>принимать</t>
+        </is>
+      </c>
+      <c r="C3133" t="inlineStr">
+        <is>
+          <t>переменная,; которая; принимает; значение</t>
+        </is>
+      </c>
+      <c r="D3133" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3133" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3134">
+      <c r="A3134" t="inlineStr">
+        <is>
+          <t>добавить</t>
+        </is>
+      </c>
+      <c r="C3134" t="inlineStr">
+        <is>
+          <t>налог; на; добавленную; стоимость</t>
+        </is>
+      </c>
+      <c r="D3134" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3134" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3135">
+      <c r="A3135" t="inlineStr">
+        <is>
+          <t>добавить</t>
+        </is>
+      </c>
+      <c r="C3135" t="inlineStr">
+        <is>
+          <t>высокая; доля; добавленной; стоимости</t>
+        </is>
+      </c>
+      <c r="D3135" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3135" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3136">
+      <c r="A3136" t="inlineStr">
+        <is>
+          <t>добавить</t>
+        </is>
+      </c>
+      <c r="C3136" t="inlineStr">
+        <is>
+          <t>формирование; цепочек; добавленной; стоимости</t>
+        </is>
+      </c>
+      <c r="D3136" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3136" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3137">
+      <c r="A3137" t="inlineStr">
+        <is>
+          <t>добавить</t>
+        </is>
+      </c>
+      <c r="C3137" t="inlineStr">
+        <is>
+          <t>структура; валовой; добавленной; стоимости</t>
+        </is>
+      </c>
+      <c r="D3137" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3137" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
+        </is>
+      </c>
+    </row>
+    <row r="3138">
+      <c r="A3138" t="inlineStr">
+        <is>
+          <t>использовать</t>
+        </is>
+      </c>
+      <c r="C3138" t="inlineStr">
+        <is>
+          <t>доля; организаций; использующих; интернет</t>
+        </is>
+      </c>
+      <c r="D3138" t="inlineStr">
+        <is>
+          <t>Поставьте слова в правильном порядке:</t>
+        </is>
+      </c>
+      <c r="E3138" t="inlineStr">
+        <is>
+          <t>Упорядочить слова</t>
         </is>
       </c>
     </row>

</xml_diff>